<commit_message>
added functions to replace "colortools" removed dependency on "colortools"
</commit_message>
<xml_diff>
--- a/inst/extdata/minimal_example_excel_template2.xlsx
+++ b/inst/extdata/minimal_example_excel_template2.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au530301_uni_au_dk/Documents/Vedhæftede filer/THJ LAB/Projects/seqNdisplayR/seqNdisplayR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{1B654877-CCA1-694D-A60D-7D0FB1EC189A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73D38806-892B-3645-9AA3-41D25E8F22C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D37F90C2-3F1C-214B-8B60-61C70DBC082A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="460" windowWidth="28800" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="500" windowWidth="35260" windowHeight="21900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Samples" sheetId="1" r:id="rId1"/>
+    <sheet name="SAMPLES" sheetId="1" r:id="rId1"/>
+    <sheet name="ANNOTATIONS" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
   <si>
     <t>strand</t>
   </si>
@@ -34,6 +45,9 @@
     <t>batch</t>
   </si>
   <si>
+    <t>3-seq</t>
+  </si>
+  <si>
     <t>L_EGFP_rep1_tt_corr_ff_noJncReads_plus.bw</t>
   </si>
   <si>
@@ -91,6 +105,15 @@
     <t>color</t>
   </si>
   <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>collapsed2</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
     <t>ChIP-seq</t>
   </si>
   <si>
@@ -118,6 +141,51 @@
     <t>subgroup_4</t>
   </si>
   <si>
+    <t>siGFP_xPAP_in_batch1_plus.bw</t>
+  </si>
+  <si>
+    <t>siGFP_xPAP_in_batch1_minus.bw</t>
+  </si>
+  <si>
+    <t>siGFP_xPAP_in_batch2_plus.bw</t>
+  </si>
+  <si>
+    <t>siGFP_xPAP_in_batch2_minus.bw</t>
+  </si>
+  <si>
+    <t>siGFP_xPAP_in_batch3_plus.bw</t>
+  </si>
+  <si>
+    <t>siGFP_xPAP_in_batch3_minus.bw</t>
+  </si>
+  <si>
+    <t>siRRP40_xPAP_in_batch1_plus.bw</t>
+  </si>
+  <si>
+    <t>siRRP40_xPAP_in_batch1_minus.bw</t>
+  </si>
+  <si>
+    <t>siRRP40_xPAP_in_batch3_plus.bw</t>
+  </si>
+  <si>
+    <t>siRRP40_xPAP_in_batch3_minus.bw</t>
+  </si>
+  <si>
+    <t>feature_names_above</t>
+  </si>
+  <si>
+    <t>incl_feature_brackets</t>
+  </si>
+  <si>
+    <t>incl_feature_shadings</t>
+  </si>
+  <si>
+    <t>incl_feature_names</t>
+  </si>
+  <si>
+    <t>in-house</t>
+  </si>
+  <si>
     <t>siCTRL</t>
   </si>
   <si>
@@ -142,6 +210,24 @@
     <t>RNAPII</t>
   </si>
   <si>
+    <t>ChIP-peaks</t>
+  </si>
+  <si>
+    <t>annot_cols</t>
+  </si>
+  <si>
+    <t>annotation_packing</t>
+  </si>
+  <si>
+    <t>annotation_name</t>
+  </si>
+  <si>
+    <t>annotation_file</t>
+  </si>
+  <si>
+    <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/tracks/HeLa_3pseq/</t>
+  </si>
+  <si>
     <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/tracks/HeLa_TTseq/</t>
   </si>
   <si>
@@ -149,13 +235,25 @@
   </si>
   <si>
     <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/tracks/HeLa_ChIPseq/</t>
+  </si>
+  <si>
+    <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/annotations/HeLa_major_isoform_hg38_gc34.bed</t>
+  </si>
+  <si>
+    <t>http://genome-ftp.mbg.au.dk/public/THJ/seqNdisplayR/examples/annotations/RNAPII_ChIP_peaks.bed</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -179,6 +277,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -230,7 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -239,6 +345,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -563,32 +678,34 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="89.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="76.33203125" customWidth="1"/>
+    <col min="4" max="4" width="79.5" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -597,52 +714,52 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -654,10 +771,10 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
@@ -669,10 +786,10 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -682,245 +799,539 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
         <v>14</v>
       </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="H22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
         <v>17</v>
       </c>
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
         <v>21</v>
       </c>
-      <c r="E17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19">
+      <c r="E28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_TTseq/" xr:uid="{B71FE05B-4E94-204C-8212-126A2EC25BF0}"/>
-    <hyperlink ref="C10" r:id="rId2" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_RNAseq/" xr:uid="{CE081A57-03EB-8545-9FF6-ED515FC84E88}"/>
-    <hyperlink ref="C18" r:id="rId3" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_ChIPseq/" xr:uid="{789F8E65-1649-D945-A802-9480409ED443}"/>
+    <hyperlink ref="C14" r:id="rId1" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_TTseq/" xr:uid="{B71FE05B-4E94-204C-8212-126A2EC25BF0}"/>
+    <hyperlink ref="C22" r:id="rId2" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_RNAseq/" xr:uid="{CE081A57-03EB-8545-9FF6-ED515FC84E88}"/>
+    <hyperlink ref="C30" r:id="rId3" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_ChIPseq/" xr:uid="{789F8E65-1649-D945-A802-9480409ED443}"/>
+    <hyperlink ref="C2" r:id="rId4" display="http://genome-ftp.mbg.au.dk/public/THJ/Seq2PlotR/examples/tracks/HeLa_3pseq/" xr:uid="{23D21FA5-27C9-004E-8822-26FC139E280E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="99" customWidth="1"/>
+    <col min="3" max="8" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0E8D3FEE-72F8-1046-A9AE-1D9A8532B73D}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{EB2690FB-ABD6-9A4A-BE8E-A0D4FBFA8EDD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>